<commit_message>
upload process and insertion, and small fix to visual and validation
</commit_message>
<xml_diff>
--- a/html/templates/occurrences.xlsx
+++ b/html/templates/occurrences.xlsx
@@ -207,39 +207,44 @@
   </sheetPr>
   <dimension ref="A1:AE1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB1" activeCellId="0" sqref="AB1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W1" activeCellId="0" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4331983805668"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6315789473684"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2105263157895"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5263157894737"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="5.76923076923077"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="5.87854251012146"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.6963562753036"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.0971659919028"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.5748987854251"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.67611336032389"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.2105263157895"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.6275303643725"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.78542510121457"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="4.60728744939271"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.29959514170041"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="3.97165991902834"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="7.03238866396761"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="11.4777327935223"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.2064777327935"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="6.40485829959514"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="14.5384615384615"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="13.3765182186235"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.331983805668"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.51821862348178"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9271255060729"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2631578947368"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0323886639676"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3765182186235"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.995951417004"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.31174089068826"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.42914979757085"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.3765182186235"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.1255060728745"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.5222672064777"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.17004048583"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.8178137651822"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.0404858299595"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.497975708502"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.5060728744939"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="4.88663967611336"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.75708502024292"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="4.33603238866397"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="7.63967611336032"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.2672064777328"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.497975708502"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="7.09311740890688"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="16.0161943319838"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="14.582995951417"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.3400809716599"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.8866396761134"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="11.9392712550607"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="10.0607287449393"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="18.4453441295547"/>
+    <col collapsed="false" hidden="false" max="1025" min="32" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>